<commit_message>
arrumando linha exist ok=true
</commit_message>
<xml_diff>
--- a/relacao_honorarios.xlsx
+++ b/relacao_honorarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logika\Downloads\Projeto Honorarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hillebrande\Documents\Project\Office-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BFADFD-C984-4C82-BDF9-B8D6B522B1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8493672C-F0E1-450C-BBA8-D72BD012778B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="honorario" sheetId="1" r:id="rId1"/>
@@ -1061,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1160,9 +1160,6 @@
     <xf numFmtId="17" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1193,6 +1190,13 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1502,16 +1506,16 @@
   <dimension ref="A1:AA246"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA93" sqref="AA93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="39" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="16" bestFit="1" customWidth="1"/>
@@ -1525,14 +1529,14 @@
     <col min="16" max="16" width="3" style="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" style="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" style="41" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="44" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.85546875" style="46" bestFit="1" customWidth="1"/>
     <col min="28" max="105" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1598,7 +1602,7 @@
       <c r="U1" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="V1" s="43" t="s">
+      <c r="V1" s="42" t="s">
         <v>167</v>
       </c>
       <c r="W1" s="22" t="s">
@@ -1613,7 +1617,7 @@
       <c r="Z1" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="AA1" s="22" t="s">
+      <c r="AA1" s="45" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1647,7 +1651,7 @@
       <c r="S2" s="25"/>
       <c r="T2" s="26"/>
       <c r="U2" s="24"/>
-      <c r="V2" s="44">
+      <c r="V2" s="43">
         <f>C2+E2+G2+I2+K2+M2+O2+Q2+S2</f>
         <v>706</v>
       </c>
@@ -1684,12 +1688,12 @@
       <c r="S3" s="25"/>
       <c r="T3" s="26"/>
       <c r="U3" s="24"/>
-      <c r="V3" s="44">
+      <c r="V3" s="43">
         <v>2118</v>
       </c>
       <c r="X3" s="31"/>
       <c r="Y3" s="31"/>
-      <c r="AA3" t="s">
+      <c r="AA3" s="46" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1723,7 +1727,7 @@
       <c r="S4" s="25"/>
       <c r="T4" s="26"/>
       <c r="U4" s="24"/>
-      <c r="V4" s="44">
+      <c r="V4" s="43">
         <f t="shared" ref="V4:V35" si="0">C4+E4+G4+I4+K4+M4+O4+Q4+S4</f>
         <v>320</v>
       </c>
@@ -1732,7 +1736,7 @@
       <c r="Z4" t="s">
         <v>172</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="46" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1766,7 +1770,7 @@
       <c r="S5" s="25"/>
       <c r="T5" s="26"/>
       <c r="U5" s="24"/>
-      <c r="V5" s="44">
+      <c r="V5" s="43">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>172</v>
       </c>
       <c r="Y5" s="31"/>
-      <c r="AA5" t="s">
+      <c r="AA5" s="46" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1808,13 +1812,13 @@
       <c r="S6" s="25"/>
       <c r="T6" s="26"/>
       <c r="U6" s="24"/>
-      <c r="V6" s="44">
+      <c r="V6" s="43">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
       <c r="X6" s="31"/>
       <c r="Y6" s="31"/>
-      <c r="AA6" t="s">
+      <c r="AA6" s="46" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1848,7 +1852,7 @@
       <c r="S7" s="25"/>
       <c r="T7" s="26"/>
       <c r="U7" s="24"/>
-      <c r="V7" s="44">
+      <c r="V7" s="43">
         <f t="shared" si="0"/>
         <v>990</v>
       </c>
@@ -1857,7 +1861,7 @@
       <c r="Z7" t="s">
         <v>172</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7" s="46" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1891,13 +1895,13 @@
       <c r="S8" s="25"/>
       <c r="T8" s="26"/>
       <c r="U8" s="24"/>
-      <c r="V8" s="44">
+      <c r="V8" s="43">
         <f t="shared" si="0"/>
         <v>353</v>
       </c>
       <c r="X8" s="31"/>
       <c r="Y8" s="31"/>
-      <c r="AA8" t="s">
+      <c r="AA8" s="46" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1931,7 +1935,7 @@
       <c r="S9" s="25"/>
       <c r="T9" s="26"/>
       <c r="U9" s="24"/>
-      <c r="V9" s="44">
+      <c r="V9" s="43">
         <f t="shared" si="0"/>
         <v>1095</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>172</v>
       </c>
       <c r="Y9" s="31"/>
-      <c r="AA9" t="s">
+      <c r="AA9" s="46" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1974,7 +1978,7 @@
       <c r="S10" s="25"/>
       <c r="T10" s="26"/>
       <c r="U10" s="24"/>
-      <c r="V10" s="44">
+      <c r="V10" s="43">
         <f t="shared" si="0"/>
         <v>1412</v>
       </c>
@@ -1982,7 +1986,7 @@
         <v>172</v>
       </c>
       <c r="Y10" s="31"/>
-      <c r="AA10" t="s">
+      <c r="AA10" s="46" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2017,7 +2021,7 @@
       <c r="S11" s="25"/>
       <c r="T11" s="26"/>
       <c r="U11" s="24"/>
-      <c r="V11" s="44">
+      <c r="V11" s="43">
         <f t="shared" si="0"/>
         <v>706</v>
       </c>
@@ -2025,7 +2029,7 @@
         <v>172</v>
       </c>
       <c r="Y11" s="31"/>
-      <c r="AA11" t="s">
+      <c r="AA11" s="46" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2060,7 +2064,7 @@
       <c r="S12" s="25"/>
       <c r="T12" s="26"/>
       <c r="U12" s="24"/>
-      <c r="V12" s="44">
+      <c r="V12" s="43">
         <f t="shared" si="0"/>
         <v>1170</v>
       </c>
@@ -2069,7 +2073,7 @@
       <c r="Z12" t="s">
         <v>172</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AA12" s="46" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2104,7 +2108,7 @@
       <c r="S13" s="25"/>
       <c r="T13" s="26"/>
       <c r="U13" s="24"/>
-      <c r="V13" s="44">
+      <c r="V13" s="43">
         <f t="shared" si="0"/>
         <v>423</v>
       </c>
@@ -2113,7 +2117,7 @@
       <c r="Z13" t="s">
         <v>172</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13" s="46" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2148,7 +2152,7 @@
       <c r="S14" s="25"/>
       <c r="T14" s="26"/>
       <c r="U14" s="24"/>
-      <c r="V14" s="44">
+      <c r="V14" s="43">
         <f t="shared" si="0"/>
         <v>353</v>
       </c>
@@ -2157,7 +2161,7 @@
       <c r="Z14" t="s">
         <v>172</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14" s="46" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2196,7 +2200,7 @@
       <c r="U15" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="V15" s="44">
+      <c r="V15" s="43">
         <f t="shared" si="0"/>
         <v>1422</v>
       </c>
@@ -2207,7 +2211,7 @@
         <v>172</v>
       </c>
       <c r="Y15" s="31"/>
-      <c r="AA15" t="s">
+      <c r="AA15" s="46" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2242,7 +2246,7 @@
       <c r="S16" s="25"/>
       <c r="T16" s="26"/>
       <c r="U16" s="24"/>
-      <c r="V16" s="44">
+      <c r="V16" s="43">
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
@@ -2251,7 +2255,7 @@
       <c r="Z16" t="s">
         <v>172</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AA16" s="46" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2286,7 +2290,7 @@
       <c r="S17" s="25"/>
       <c r="T17" s="26"/>
       <c r="U17" s="24"/>
-      <c r="V17" s="44">
+      <c r="V17" s="43">
         <f t="shared" si="0"/>
         <v>990</v>
       </c>
@@ -2295,7 +2299,7 @@
       <c r="Z17" t="s">
         <v>172</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AA17" s="46" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2330,13 +2334,13 @@
       <c r="S18" s="25"/>
       <c r="T18" s="26"/>
       <c r="U18" s="24"/>
-      <c r="V18" s="44">
+      <c r="V18" s="43">
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
       <c r="X18" s="31"/>
       <c r="Y18" s="31"/>
-      <c r="AA18" t="s">
+      <c r="AA18" s="46" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2371,7 +2375,7 @@
       <c r="S19" s="25"/>
       <c r="T19" s="26"/>
       <c r="U19" s="24"/>
-      <c r="V19" s="44">
+      <c r="V19" s="43">
         <f t="shared" si="0"/>
         <v>650</v>
       </c>
@@ -2379,7 +2383,7 @@
         <v>172</v>
       </c>
       <c r="Y19" s="31"/>
-      <c r="AA19" t="s">
+      <c r="AA19" s="46" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2414,7 +2418,7 @@
       <c r="S20" s="25"/>
       <c r="T20" s="26"/>
       <c r="U20" s="24"/>
-      <c r="V20" s="44">
+      <c r="V20" s="43">
         <f t="shared" si="0"/>
         <v>706</v>
       </c>
@@ -2422,7 +2426,7 @@
         <v>172</v>
       </c>
       <c r="Y20" s="31"/>
-      <c r="AA20" t="s">
+      <c r="AA20" s="46" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2457,13 +2461,13 @@
       <c r="S21" s="25"/>
       <c r="T21" s="33"/>
       <c r="U21" s="24"/>
-      <c r="V21" s="44">
+      <c r="V21" s="43">
         <f t="shared" si="0"/>
         <v>706</v>
       </c>
       <c r="X21" s="31"/>
       <c r="Y21" s="31"/>
-      <c r="AA21" t="s">
+      <c r="AA21" s="46" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2497,13 +2501,13 @@
       <c r="S22" s="25"/>
       <c r="T22" s="26"/>
       <c r="U22" s="24"/>
-      <c r="V22" s="44">
+      <c r="V22" s="43">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
       <c r="X22" s="31"/>
       <c r="Y22" s="31"/>
-      <c r="AA22" t="s">
+      <c r="AA22" s="46" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2538,7 +2542,7 @@
       <c r="S23" s="25"/>
       <c r="T23" s="29"/>
       <c r="U23" s="24"/>
-      <c r="V23" s="44">
+      <c r="V23" s="43">
         <f t="shared" si="0"/>
         <v>706</v>
       </c>
@@ -2546,7 +2550,7 @@
       <c r="Y23" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AA23" s="46" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2581,7 +2585,7 @@
       <c r="S24" s="25"/>
       <c r="T24" s="26"/>
       <c r="U24" s="24"/>
-      <c r="V24" s="44">
+      <c r="V24" s="43">
         <f t="shared" si="0"/>
         <v>2118</v>
       </c>
@@ -2589,7 +2593,7 @@
         <v>172</v>
       </c>
       <c r="Y24" s="31"/>
-      <c r="AA24" t="s">
+      <c r="AA24" s="46" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2624,13 +2628,13 @@
       <c r="S25" s="25"/>
       <c r="T25" s="26"/>
       <c r="U25" s="26"/>
-      <c r="V25" s="44">
+      <c r="V25" s="43">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="X25" s="31"/>
       <c r="Y25" s="31"/>
-      <c r="AA25" t="s">
+      <c r="AA25" s="46" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2665,7 +2669,7 @@
       <c r="S26" s="25"/>
       <c r="T26" s="26"/>
       <c r="U26" s="24"/>
-      <c r="V26" s="44">
+      <c r="V26" s="43">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
@@ -2706,7 +2710,7 @@
       <c r="S27" s="25"/>
       <c r="T27" s="26"/>
       <c r="U27" s="24"/>
-      <c r="V27" s="44">
+      <c r="V27" s="43">
         <f t="shared" si="0"/>
         <v>420</v>
       </c>
@@ -2714,7 +2718,7 @@
         <v>172</v>
       </c>
       <c r="Y27" s="31"/>
-      <c r="AA27" t="s">
+      <c r="AA27" s="46" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2749,13 +2753,13 @@
       <c r="S28" s="25"/>
       <c r="T28" s="26"/>
       <c r="U28" s="24"/>
-      <c r="V28" s="44">
+      <c r="V28" s="43">
         <f t="shared" si="0"/>
         <v>353</v>
       </c>
       <c r="X28" s="31"/>
       <c r="Y28" s="31"/>
-      <c r="AA28" t="s">
+      <c r="AA28" s="46" t="s">
         <v>203</v>
       </c>
     </row>
@@ -2790,13 +2794,13 @@
       <c r="S29" s="25"/>
       <c r="T29" s="26"/>
       <c r="U29" s="24"/>
-      <c r="V29" s="44">
+      <c r="V29" s="43">
         <f t="shared" si="0"/>
         <v>353</v>
       </c>
       <c r="X29" s="31"/>
       <c r="Y29" s="31"/>
-      <c r="AA29" t="s">
+      <c r="AA29" s="46" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2831,13 +2835,13 @@
       <c r="S30" s="25"/>
       <c r="T30" s="26"/>
       <c r="U30" s="24"/>
-      <c r="V30" s="44">
+      <c r="V30" s="43">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="X30" s="31"/>
       <c r="Y30" s="31"/>
-      <c r="AA30" t="s">
+      <c r="AA30" s="46" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2872,7 +2876,7 @@
       <c r="S31" s="25"/>
       <c r="T31" s="26"/>
       <c r="U31" s="24"/>
-      <c r="V31" s="44">
+      <c r="V31" s="43">
         <f t="shared" si="0"/>
         <v>2118</v>
       </c>
@@ -2881,7 +2885,7 @@
       <c r="Z31" t="s">
         <v>172</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AA31" s="46" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2916,7 +2920,7 @@
       <c r="S32" s="25"/>
       <c r="T32" s="26"/>
       <c r="U32" s="24"/>
-      <c r="V32" s="44">
+      <c r="V32" s="43">
         <f t="shared" si="0"/>
         <v>1412</v>
       </c>
@@ -2925,7 +2929,7 @@
       <c r="Z32" t="s">
         <v>172</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AA32" s="46" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2960,13 +2964,13 @@
       <c r="S33" s="25"/>
       <c r="T33" s="26"/>
       <c r="U33" s="24"/>
-      <c r="V33" s="44">
+      <c r="V33" s="43">
         <f t="shared" si="0"/>
         <v>405</v>
       </c>
       <c r="X33" s="31"/>
       <c r="Y33" s="31"/>
-      <c r="AA33" t="s">
+      <c r="AA33" s="46" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3001,13 +3005,13 @@
       <c r="S34" s="25"/>
       <c r="T34" s="26"/>
       <c r="U34" s="24"/>
-      <c r="V34" s="44">
+      <c r="V34" s="43">
         <f t="shared" si="0"/>
         <v>706</v>
       </c>
       <c r="X34" s="31"/>
       <c r="Y34" s="31"/>
-      <c r="AA34" t="s">
+      <c r="AA34" s="46" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3042,13 +3046,13 @@
       <c r="S35" s="25"/>
       <c r="T35" s="26"/>
       <c r="U35" s="24"/>
-      <c r="V35" s="44">
+      <c r="V35" s="43">
         <f t="shared" si="0"/>
         <v>353</v>
       </c>
       <c r="X35" s="31"/>
       <c r="Y35" s="31"/>
-      <c r="AA35" s="34" t="s">
+      <c r="AA35" s="47" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3083,7 +3087,7 @@
       <c r="S36" s="25"/>
       <c r="T36" s="26"/>
       <c r="U36" s="24"/>
-      <c r="V36" s="44">
+      <c r="V36" s="43">
         <f t="shared" ref="V36:V67" si="3">C36+E36+G36+I36+K36+M36+O36+Q36+S36</f>
         <v>1412</v>
       </c>
@@ -3092,7 +3096,7 @@
       <c r="Z36" t="s">
         <v>172</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AA36" s="46" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3127,7 +3131,7 @@
       <c r="S37" s="25"/>
       <c r="T37" s="26"/>
       <c r="U37" s="24"/>
-      <c r="V37" s="44">
+      <c r="V37" s="43">
         <f t="shared" si="3"/>
         <v>353</v>
       </c>
@@ -3136,7 +3140,7 @@
       <c r="Z37" t="s">
         <v>172</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="AA37" s="46" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3171,13 +3175,13 @@
       <c r="S38" s="25"/>
       <c r="T38" s="26"/>
       <c r="U38" s="24"/>
-      <c r="V38" s="44">
+      <c r="V38" s="43">
         <f t="shared" si="3"/>
         <v>353</v>
       </c>
       <c r="X38" s="31"/>
       <c r="Y38" s="31"/>
-      <c r="AA38" t="s">
+      <c r="AA38" s="46" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3216,7 +3220,7 @@
       <c r="U39" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="V39" s="44">
+      <c r="V39" s="43">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
@@ -3224,7 +3228,7 @@
         <v>172</v>
       </c>
       <c r="Y39" s="31"/>
-      <c r="AA39" t="s">
+      <c r="AA39" s="46" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3233,7 +3237,7 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="34" t="s">
         <v>219</v>
       </c>
       <c r="C40" s="25">
@@ -3259,13 +3263,13 @@
       <c r="S40" s="25"/>
       <c r="T40" s="26"/>
       <c r="U40" s="24"/>
-      <c r="V40" s="44">
+      <c r="V40" s="43">
         <f t="shared" si="3"/>
         <v>706</v>
       </c>
       <c r="X40" s="31"/>
       <c r="Y40" s="31"/>
-      <c r="AA40" t="s">
+      <c r="AA40" s="46" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3300,13 +3304,13 @@
       <c r="S41" s="25"/>
       <c r="T41" s="26"/>
       <c r="U41" s="24"/>
-      <c r="V41" s="44">
+      <c r="V41" s="43">
         <f t="shared" si="3"/>
         <v>706</v>
       </c>
       <c r="X41" s="31"/>
       <c r="Y41" s="31"/>
-      <c r="AA41" t="s">
+      <c r="AA41" s="46" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3345,7 +3349,7 @@
       <c r="U42" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="V42" s="44">
+      <c r="V42" s="43">
         <f t="shared" si="3"/>
         <v>2964</v>
       </c>
@@ -3353,7 +3357,7 @@
         <v>172</v>
       </c>
       <c r="Y42" s="31"/>
-      <c r="AA42" t="s">
+      <c r="AA42" s="46" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3362,7 +3366,7 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="35" t="s">
         <v>66</v>
       </c>
       <c r="C43" s="25">
@@ -3388,13 +3392,13 @@
       <c r="S43" s="25"/>
       <c r="T43" s="26"/>
       <c r="U43" s="24"/>
-      <c r="V43" s="44">
+      <c r="V43" s="43">
         <f t="shared" si="3"/>
         <v>706</v>
       </c>
       <c r="X43" s="31"/>
       <c r="Y43" s="31"/>
-      <c r="AA43" t="s">
+      <c r="AA43" s="46" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3429,13 +3433,13 @@
       <c r="S44" s="25"/>
       <c r="T44" s="27"/>
       <c r="U44" s="24"/>
-      <c r="V44" s="44">
+      <c r="V44" s="43">
         <f t="shared" si="3"/>
         <v>706</v>
       </c>
       <c r="X44" s="31"/>
       <c r="Y44" s="31"/>
-      <c r="AA44" t="s">
+      <c r="AA44" s="46" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3474,13 +3478,13 @@
       <c r="U45" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="V45" s="44">
+      <c r="V45" s="43">
         <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="X45" s="31"/>
       <c r="Y45" s="31"/>
-      <c r="AA45" t="s">
+      <c r="AA45" s="46" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3515,7 +3519,7 @@
       <c r="S46" s="25"/>
       <c r="T46" s="26"/>
       <c r="U46" s="24"/>
-      <c r="V46" s="44">
+      <c r="V46" s="43">
         <f t="shared" si="3"/>
         <v>2118</v>
       </c>
@@ -3524,7 +3528,7 @@
       <c r="Z46" t="s">
         <v>172</v>
       </c>
-      <c r="AA46" t="s">
+      <c r="AA46" s="46" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3559,7 +3563,7 @@
       <c r="S47" s="25"/>
       <c r="T47" s="26"/>
       <c r="U47" s="24"/>
-      <c r="V47" s="44">
+      <c r="V47" s="43">
         <f t="shared" si="3"/>
         <v>170</v>
       </c>
@@ -3599,7 +3603,7 @@
       <c r="S48" s="25"/>
       <c r="T48" s="26"/>
       <c r="U48" s="24"/>
-      <c r="V48" s="44">
+      <c r="V48" s="43">
         <f t="shared" si="3"/>
         <v>1412</v>
       </c>
@@ -3607,7 +3611,7 @@
         <v>172</v>
       </c>
       <c r="Y48" s="31"/>
-      <c r="AA48" t="s">
+      <c r="AA48" s="46" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3642,13 +3646,13 @@
       <c r="S49" s="25"/>
       <c r="T49" s="26"/>
       <c r="U49" s="24"/>
-      <c r="V49" s="44">
+      <c r="V49" s="43">
         <f t="shared" si="3"/>
         <v>353</v>
       </c>
       <c r="X49" s="31"/>
       <c r="Y49" s="31"/>
-      <c r="AA49" t="s">
+      <c r="AA49" s="46" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3683,13 +3687,13 @@
       <c r="S50" s="25"/>
       <c r="T50" s="26"/>
       <c r="U50" s="24"/>
-      <c r="V50" s="44">
+      <c r="V50" s="43">
         <f t="shared" si="3"/>
         <v>1412</v>
       </c>
       <c r="X50" s="31"/>
       <c r="Y50" s="31"/>
-      <c r="AA50" t="s">
+      <c r="AA50" s="46" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3724,7 +3728,7 @@
       <c r="S51" s="25"/>
       <c r="T51" s="26"/>
       <c r="U51" s="24"/>
-      <c r="V51" s="44">
+      <c r="V51" s="43">
         <f t="shared" si="3"/>
         <v>706</v>
       </c>
@@ -3764,13 +3768,13 @@
       <c r="S52" s="25"/>
       <c r="T52" s="26"/>
       <c r="U52" s="24"/>
-      <c r="V52" s="44">
+      <c r="V52" s="43">
         <f t="shared" si="3"/>
         <v>353</v>
       </c>
       <c r="X52" s="31"/>
       <c r="Y52" s="31"/>
-      <c r="AA52" t="s">
+      <c r="AA52" s="46" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3809,7 +3813,7 @@
       <c r="U53" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="V53" s="44">
+      <c r="V53" s="43">
         <f t="shared" si="3"/>
         <v>1422</v>
       </c>
@@ -3817,7 +3821,7 @@
         <v>172</v>
       </c>
       <c r="Y53" s="31"/>
-      <c r="AA53" t="s">
+      <c r="AA53" s="46" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3852,13 +3856,13 @@
       <c r="S54" s="25"/>
       <c r="T54" s="26"/>
       <c r="U54" s="24"/>
-      <c r="V54" s="44">
+      <c r="V54" s="43">
         <f t="shared" si="3"/>
         <v>1130</v>
       </c>
       <c r="X54" s="31"/>
       <c r="Y54" s="31"/>
-      <c r="AA54" t="s">
+      <c r="AA54" s="46" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3893,7 +3897,7 @@
       <c r="S55" s="25"/>
       <c r="T55" s="26"/>
       <c r="U55" s="24"/>
-      <c r="V55" s="44">
+      <c r="V55" s="43">
         <f t="shared" si="3"/>
         <v>580</v>
       </c>
@@ -3901,7 +3905,7 @@
         <v>172</v>
       </c>
       <c r="Y55" s="31"/>
-      <c r="AA55" t="s">
+      <c r="AA55" s="46" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3936,7 +3940,7 @@
       <c r="S56" s="25"/>
       <c r="T56" s="26"/>
       <c r="U56" s="24"/>
-      <c r="V56" s="44">
+      <c r="V56" s="43">
         <f t="shared" si="3"/>
         <v>2118</v>
       </c>
@@ -3945,7 +3949,7 @@
       <c r="Z56" t="s">
         <v>172</v>
       </c>
-      <c r="AA56" t="s">
+      <c r="AA56" s="46" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3980,7 +3984,7 @@
       <c r="S57" s="25"/>
       <c r="T57" s="26"/>
       <c r="U57" s="24"/>
-      <c r="V57" s="44">
+      <c r="V57" s="43">
         <f t="shared" si="3"/>
         <v>1412</v>
       </c>
@@ -3988,7 +3992,7 @@
       <c r="Y57" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="AA57" t="s">
+      <c r="AA57" s="46" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4023,7 +4027,7 @@
       <c r="S58" s="25"/>
       <c r="T58" s="26"/>
       <c r="U58" s="24"/>
-      <c r="V58" s="44">
+      <c r="V58" s="43">
         <f t="shared" si="3"/>
         <v>1412</v>
       </c>
@@ -4031,7 +4035,7 @@
       <c r="Y58" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="AA58" t="s">
+      <c r="AA58" s="46" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4066,13 +4070,13 @@
       <c r="S59" s="25"/>
       <c r="T59" s="26"/>
       <c r="U59" s="24"/>
-      <c r="V59" s="44">
+      <c r="V59" s="43">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
       <c r="X59" s="31"/>
       <c r="Y59" s="31"/>
-      <c r="AA59" t="s">
+      <c r="AA59" s="46" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4107,13 +4111,13 @@
       <c r="S60" s="25"/>
       <c r="T60" s="26"/>
       <c r="U60" s="24"/>
-      <c r="V60" s="44">
+      <c r="V60" s="43">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="X60" s="31"/>
       <c r="Y60" s="31"/>
-      <c r="AA60" t="s">
+      <c r="AA60" s="46" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4148,7 +4152,7 @@
       <c r="S61" s="25"/>
       <c r="T61" s="26"/>
       <c r="U61" s="24"/>
-      <c r="V61" s="44">
+      <c r="V61" s="43">
         <f t="shared" si="3"/>
         <v>890</v>
       </c>
@@ -4189,7 +4193,7 @@
       <c r="S62" s="25"/>
       <c r="T62" s="27"/>
       <c r="U62" s="24"/>
-      <c r="V62" s="44">
+      <c r="V62" s="43">
         <f t="shared" si="3"/>
         <v>2824</v>
       </c>
@@ -4198,7 +4202,7 @@
       <c r="Z62" t="s">
         <v>172</v>
       </c>
-      <c r="AA62" t="s">
+      <c r="AA62" s="46" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4233,7 +4237,7 @@
       <c r="S63" s="25"/>
       <c r="T63" s="26"/>
       <c r="U63" s="24"/>
-      <c r="V63" s="44">
+      <c r="V63" s="43">
         <f t="shared" si="3"/>
         <v>529</v>
       </c>
@@ -4242,7 +4246,7 @@
       <c r="Z63" t="s">
         <v>172</v>
       </c>
-      <c r="AA63" t="s">
+      <c r="AA63" s="46" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4277,7 +4281,7 @@
       <c r="S64" s="25"/>
       <c r="T64" s="26"/>
       <c r="U64" s="24"/>
-      <c r="V64" s="44">
+      <c r="V64" s="43">
         <f t="shared" si="3"/>
         <v>4236</v>
       </c>
@@ -4286,7 +4290,7 @@
       <c r="Z64" t="s">
         <v>172</v>
       </c>
-      <c r="AA64" t="s">
+      <c r="AA64" s="46" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4321,13 +4325,13 @@
       <c r="S65" s="25"/>
       <c r="T65" s="26"/>
       <c r="U65" s="24"/>
-      <c r="V65" s="44">
+      <c r="V65" s="43">
         <f t="shared" si="3"/>
         <v>706</v>
       </c>
       <c r="X65" s="31"/>
       <c r="Y65" s="31"/>
-      <c r="AA65" t="s">
+      <c r="AA65" s="46" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4366,13 +4370,13 @@
       <c r="U66" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="V66" s="44">
+      <c r="V66" s="43">
         <f t="shared" si="3"/>
         <v>1492</v>
       </c>
       <c r="X66" s="31"/>
       <c r="Y66" s="31"/>
-      <c r="AA66" t="s">
+      <c r="AA66" s="46" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4407,13 +4411,13 @@
       <c r="S67" s="25"/>
       <c r="T67" s="26"/>
       <c r="U67" s="24"/>
-      <c r="V67" s="44">
+      <c r="V67" s="43">
         <f t="shared" si="3"/>
         <v>706</v>
       </c>
       <c r="X67" s="31"/>
       <c r="Y67" s="31"/>
-      <c r="AA67" t="s">
+      <c r="AA67" s="46" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4448,7 +4452,7 @@
       <c r="S68" s="25"/>
       <c r="T68" s="26"/>
       <c r="U68" s="24"/>
-      <c r="V68" s="44">
+      <c r="V68" s="43">
         <f t="shared" ref="V68:V95" si="5">C68+E68+G68+I68+K68+M68+O68+Q68+S68</f>
         <v>280</v>
       </c>
@@ -4457,7 +4461,7 @@
       <c r="Z68" t="s">
         <v>172</v>
       </c>
-      <c r="AA68" t="s">
+      <c r="AA68" s="46" t="s">
         <v>249</v>
       </c>
     </row>
@@ -4492,13 +4496,13 @@
       <c r="S69" s="25"/>
       <c r="T69" s="26"/>
       <c r="U69" s="24"/>
-      <c r="V69" s="44">
+      <c r="V69" s="43">
         <f t="shared" si="5"/>
         <v>353</v>
       </c>
       <c r="X69" s="31"/>
       <c r="Y69" s="31"/>
-      <c r="AA69" t="s">
+      <c r="AA69" s="46" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4533,7 +4537,7 @@
       <c r="S70" s="25"/>
       <c r="T70" s="26"/>
       <c r="U70" s="24"/>
-      <c r="V70" s="44">
+      <c r="V70" s="43">
         <f t="shared" si="5"/>
         <v>706</v>
       </c>
@@ -4542,7 +4546,7 @@
       <c r="Z70" t="s">
         <v>172</v>
       </c>
-      <c r="AA70" t="s">
+      <c r="AA70" s="46" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4577,13 +4581,13 @@
       <c r="S71" s="25"/>
       <c r="T71" s="26"/>
       <c r="U71" s="24"/>
-      <c r="V71" s="44">
+      <c r="V71" s="43">
         <f t="shared" si="5"/>
         <v>1412</v>
       </c>
       <c r="X71" s="31"/>
       <c r="Y71" s="31"/>
-      <c r="AA71" t="s">
+      <c r="AA71" s="46" t="s">
         <v>253</v>
       </c>
     </row>
@@ -4618,13 +4622,13 @@
       <c r="S72" s="25"/>
       <c r="T72" s="26"/>
       <c r="U72" s="24"/>
-      <c r="V72" s="44">
+      <c r="V72" s="43">
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
       <c r="X72" s="31"/>
       <c r="Y72" s="31"/>
-      <c r="AA72" t="s">
+      <c r="AA72" s="46" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4659,13 +4663,13 @@
       <c r="S73" s="25"/>
       <c r="T73" s="26"/>
       <c r="U73" s="24"/>
-      <c r="V73" s="44">
+      <c r="V73" s="43">
         <f t="shared" si="5"/>
         <v>926</v>
       </c>
       <c r="X73" s="31"/>
       <c r="Y73" s="31"/>
-      <c r="AA73" t="s">
+      <c r="AA73" s="46" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4700,13 +4704,13 @@
       <c r="S74" s="25"/>
       <c r="T74" s="26"/>
       <c r="U74" s="24"/>
-      <c r="V74" s="44">
+      <c r="V74" s="43">
         <f t="shared" si="5"/>
         <v>250</v>
       </c>
       <c r="X74" s="31"/>
       <c r="Y74" s="31"/>
-      <c r="AA74" t="s">
+      <c r="AA74" s="46" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4741,7 +4745,7 @@
       <c r="S75" s="25"/>
       <c r="T75" s="26"/>
       <c r="U75" s="24"/>
-      <c r="V75" s="44">
+      <c r="V75" s="43">
         <f t="shared" si="5"/>
         <v>400</v>
       </c>
@@ -4749,7 +4753,7 @@
         <v>172</v>
       </c>
       <c r="Y75" s="31"/>
-      <c r="AA75" t="s">
+      <c r="AA75" s="46" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4784,7 +4788,7 @@
       <c r="S76" s="25"/>
       <c r="T76" s="26"/>
       <c r="U76" s="24"/>
-      <c r="V76" s="44">
+      <c r="V76" s="43">
         <f t="shared" si="5"/>
         <v>250</v>
       </c>
@@ -4792,7 +4796,7 @@
         <v>172</v>
       </c>
       <c r="Y76" s="31"/>
-      <c r="AA76" t="s">
+      <c r="AA76" s="46" t="s">
         <v>258</v>
       </c>
     </row>
@@ -4827,7 +4831,7 @@
       <c r="S77" s="25"/>
       <c r="T77" s="26"/>
       <c r="U77" s="24"/>
-      <c r="V77" s="44">
+      <c r="V77" s="43">
         <f t="shared" si="5"/>
         <v>390</v>
       </c>
@@ -4836,7 +4840,7 @@
       <c r="Z77" t="s">
         <v>172</v>
       </c>
-      <c r="AA77" t="s">
+      <c r="AA77" s="46" t="s">
         <v>259</v>
       </c>
     </row>
@@ -4871,13 +4875,13 @@
       <c r="S78" s="25"/>
       <c r="T78" s="26"/>
       <c r="U78" s="24"/>
-      <c r="V78" s="44">
+      <c r="V78" s="43">
         <f t="shared" si="5"/>
         <v>706</v>
       </c>
       <c r="X78" s="31"/>
       <c r="Y78" s="31"/>
-      <c r="AA78" t="s">
+      <c r="AA78" s="46" t="s">
         <v>260</v>
       </c>
     </row>
@@ -4912,7 +4916,7 @@
       <c r="S79" s="25"/>
       <c r="T79" s="26"/>
       <c r="U79" s="24"/>
-      <c r="V79" s="44">
+      <c r="V79" s="43">
         <f t="shared" si="5"/>
         <v>706</v>
       </c>
@@ -4921,7 +4925,7 @@
       <c r="Z79" t="s">
         <v>172</v>
       </c>
-      <c r="AA79" t="s">
+      <c r="AA79" s="46" t="s">
         <v>261</v>
       </c>
     </row>
@@ -4956,7 +4960,7 @@
       <c r="S80" s="25"/>
       <c r="T80" s="26"/>
       <c r="U80" s="24"/>
-      <c r="V80" s="44">
+      <c r="V80" s="43">
         <f t="shared" si="5"/>
         <v>450</v>
       </c>
@@ -4965,7 +4969,7 @@
       <c r="Z80" t="s">
         <v>172</v>
       </c>
-      <c r="AA80" t="s">
+      <c r="AA80" s="46" t="s">
         <v>262</v>
       </c>
     </row>
@@ -5000,13 +5004,13 @@
       <c r="S81" s="25"/>
       <c r="T81" s="26"/>
       <c r="U81" s="24"/>
-      <c r="V81" s="44">
+      <c r="V81" s="43">
         <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="X81" s="31"/>
       <c r="Y81" s="31"/>
-      <c r="AA81" t="s">
+      <c r="AA81" s="46" t="s">
         <v>264</v>
       </c>
     </row>
@@ -5041,7 +5045,7 @@
       <c r="S82" s="25"/>
       <c r="T82" s="26"/>
       <c r="U82" s="24"/>
-      <c r="V82" s="44">
+      <c r="V82" s="43">
         <f t="shared" si="5"/>
         <v>706</v>
       </c>
@@ -5049,7 +5053,7 @@
         <v>172</v>
       </c>
       <c r="Y82" s="31"/>
-      <c r="AA82" t="s">
+      <c r="AA82" s="46" t="s">
         <v>265</v>
       </c>
     </row>
@@ -5084,13 +5088,13 @@
       <c r="S83" s="25"/>
       <c r="T83" s="26"/>
       <c r="U83" s="24"/>
-      <c r="V83" s="44">
+      <c r="V83" s="43">
         <f t="shared" si="5"/>
         <v>1130</v>
       </c>
       <c r="X83" s="31"/>
       <c r="Y83" s="31"/>
-      <c r="AA83" t="s">
+      <c r="AA83" s="46" t="s">
         <v>266</v>
       </c>
     </row>
@@ -5125,7 +5129,7 @@
       <c r="S84" s="25"/>
       <c r="T84" s="26"/>
       <c r="U84" s="24"/>
-      <c r="V84" s="44">
+      <c r="V84" s="43">
         <f t="shared" si="5"/>
         <v>2118</v>
       </c>
@@ -5134,7 +5138,7 @@
       <c r="Z84" t="s">
         <v>172</v>
       </c>
-      <c r="AA84" t="s">
+      <c r="AA84" s="46" t="s">
         <v>267</v>
       </c>
     </row>
@@ -5169,7 +5173,7 @@
       <c r="S85" s="25"/>
       <c r="T85" s="26"/>
       <c r="U85" s="24"/>
-      <c r="V85" s="44">
+      <c r="V85" s="43">
         <f t="shared" si="5"/>
         <v>1130</v>
       </c>
@@ -5177,7 +5181,7 @@
         <v>172</v>
       </c>
       <c r="Y85" s="31"/>
-      <c r="AA85" t="s">
+      <c r="AA85" s="46" t="s">
         <v>268</v>
       </c>
     </row>
@@ -5212,13 +5216,13 @@
       <c r="S86" s="25"/>
       <c r="T86" s="26"/>
       <c r="U86" s="24"/>
-      <c r="V86" s="44">
+      <c r="V86" s="43">
         <f t="shared" si="5"/>
         <v>580</v>
       </c>
       <c r="X86" s="31"/>
       <c r="Y86" s="31"/>
-      <c r="AA86" t="s">
+      <c r="AA86" s="46" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5253,13 +5257,13 @@
       <c r="S87" s="25"/>
       <c r="T87" s="26"/>
       <c r="U87" s="24"/>
-      <c r="V87" s="44">
+      <c r="V87" s="43">
         <f t="shared" si="5"/>
         <v>360</v>
       </c>
       <c r="X87" s="31"/>
       <c r="Y87" s="31"/>
-      <c r="AA87" t="s">
+      <c r="AA87" s="46" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5294,13 +5298,13 @@
       <c r="S88" s="25"/>
       <c r="T88" s="26"/>
       <c r="U88" s="24"/>
-      <c r="V88" s="44">
+      <c r="V88" s="43">
         <f t="shared" si="5"/>
         <v>230</v>
       </c>
       <c r="X88" s="31"/>
       <c r="Y88" s="31"/>
-      <c r="AA88" t="s">
+      <c r="AA88" s="46" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5335,13 +5339,13 @@
       <c r="S89" s="25"/>
       <c r="T89" s="26"/>
       <c r="U89" s="24"/>
-      <c r="V89" s="44">
+      <c r="V89" s="43">
         <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="X89" s="31"/>
       <c r="Y89" s="31"/>
-      <c r="AA89" t="s">
+      <c r="AA89" s="46" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5376,13 +5380,13 @@
       <c r="S90" s="25"/>
       <c r="T90" s="26"/>
       <c r="U90" s="24"/>
-      <c r="V90" s="44">
+      <c r="V90" s="43">
         <f t="shared" si="5"/>
         <v>706</v>
       </c>
       <c r="X90" s="31"/>
       <c r="Y90" s="31"/>
-      <c r="AA90" t="s">
+      <c r="AA90" s="46" t="s">
         <v>274</v>
       </c>
     </row>
@@ -5417,7 +5421,7 @@
       <c r="S91" s="25"/>
       <c r="T91" s="26"/>
       <c r="U91" s="24"/>
-      <c r="V91" s="44">
+      <c r="V91" s="43">
         <f t="shared" si="5"/>
         <v>350</v>
       </c>
@@ -5426,7 +5430,7 @@
       <c r="Z91" t="s">
         <v>172</v>
       </c>
-      <c r="AA91" t="s">
+      <c r="AA91" s="46" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5461,13 +5465,13 @@
       <c r="S92" s="25"/>
       <c r="T92" s="26"/>
       <c r="U92" s="24"/>
-      <c r="V92" s="44">
+      <c r="V92" s="43">
         <f t="shared" si="5"/>
         <v>700</v>
       </c>
       <c r="X92" s="31"/>
       <c r="Y92" s="31"/>
-      <c r="AA92" t="s">
+      <c r="AA92" s="46" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5502,13 +5506,13 @@
       <c r="S93" s="25"/>
       <c r="T93" s="26"/>
       <c r="U93" s="24"/>
-      <c r="V93" s="44">
+      <c r="V93" s="43">
         <f t="shared" si="5"/>
         <v>580</v>
       </c>
       <c r="X93" s="31"/>
       <c r="Y93" s="31"/>
-      <c r="AA93" t="s">
+      <c r="AA93" s="46" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5543,7 +5547,7 @@
       <c r="S94" s="25"/>
       <c r="T94" s="26"/>
       <c r="U94" s="24"/>
-      <c r="V94" s="44">
+      <c r="V94" s="43">
         <f t="shared" si="5"/>
         <v>1130</v>
       </c>
@@ -5552,7 +5556,7 @@
       <c r="Z94" t="s">
         <v>172</v>
       </c>
-      <c r="AA94" t="s">
+      <c r="AA94" s="46" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5587,22 +5591,22 @@
       <c r="S95" s="25"/>
       <c r="T95" s="26"/>
       <c r="U95" s="24"/>
-      <c r="V95" s="44">
+      <c r="V95" s="43">
         <f t="shared" si="5"/>
         <v>580</v>
       </c>
       <c r="X95" s="31"/>
       <c r="Y95" s="31"/>
-      <c r="AA95" t="s">
+      <c r="AA95" s="46" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:27" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="23"/>
-      <c r="B96" s="37" t="s">
+      <c r="B96" s="36" t="s">
         <v>279</v>
       </c>
-      <c r="C96" s="38">
+      <c r="C96" s="37">
         <f>SUM(C2:C95)</f>
         <v>81301</v>
       </c>
@@ -5627,460 +5631,460 @@
       </c>
       <c r="T96" s="26"/>
       <c r="U96" s="24"/>
-      <c r="V96" s="44">
+      <c r="V96" s="43">
         <f>C96+F96+H96+J96+P96+R96+S96+M96+E96</f>
         <v>81210</v>
       </c>
     </row>
     <row r="97" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K97" s="41"/>
+      <c r="K97" s="40"/>
     </row>
     <row r="98" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K98" s="41"/>
+      <c r="K98" s="40"/>
     </row>
     <row r="99" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K99" s="41"/>
+      <c r="K99" s="40"/>
     </row>
     <row r="100" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K100" s="41"/>
+      <c r="K100" s="40"/>
     </row>
     <row r="101" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K101" s="41"/>
+      <c r="K101" s="40"/>
     </row>
     <row r="102" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K102" s="41"/>
+      <c r="K102" s="40"/>
     </row>
     <row r="103" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K103" s="41"/>
+      <c r="K103" s="40"/>
     </row>
     <row r="104" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K104" s="41"/>
+      <c r="K104" s="40"/>
     </row>
     <row r="105" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K105" s="41"/>
+      <c r="K105" s="40"/>
     </row>
     <row r="106" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K106" s="41"/>
+      <c r="K106" s="40"/>
     </row>
     <row r="107" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K107" s="41"/>
+      <c r="K107" s="40"/>
     </row>
     <row r="108" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K108" s="41"/>
+      <c r="K108" s="40"/>
     </row>
     <row r="109" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K109" s="41"/>
+      <c r="K109" s="40"/>
     </row>
     <row r="110" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K110" s="41"/>
+      <c r="K110" s="40"/>
     </row>
     <row r="111" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K111" s="41"/>
+      <c r="K111" s="40"/>
     </row>
     <row r="112" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K112" s="41"/>
+      <c r="K112" s="40"/>
     </row>
     <row r="113" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K113" s="41"/>
+      <c r="K113" s="40"/>
     </row>
     <row r="114" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K114" s="41"/>
+      <c r="K114" s="40"/>
     </row>
     <row r="115" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K115" s="41"/>
+      <c r="K115" s="40"/>
     </row>
     <row r="116" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K116" s="41"/>
+      <c r="K116" s="40"/>
     </row>
     <row r="117" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K117" s="41"/>
+      <c r="K117" s="40"/>
     </row>
     <row r="118" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K118" s="41"/>
+      <c r="K118" s="40"/>
     </row>
     <row r="119" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K119" s="41"/>
+      <c r="K119" s="40"/>
     </row>
     <row r="120" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K120" s="41"/>
+      <c r="K120" s="40"/>
     </row>
     <row r="121" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K121" s="41"/>
+      <c r="K121" s="40"/>
     </row>
     <row r="122" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K122" s="41"/>
+      <c r="K122" s="40"/>
     </row>
     <row r="123" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K123" s="41"/>
+      <c r="K123" s="40"/>
     </row>
     <row r="124" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K124" s="41"/>
+      <c r="K124" s="40"/>
     </row>
     <row r="125" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K125" s="41"/>
+      <c r="K125" s="40"/>
     </row>
     <row r="126" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K126" s="41"/>
+      <c r="K126" s="40"/>
     </row>
     <row r="127" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K127" s="41"/>
+      <c r="K127" s="40"/>
     </row>
     <row r="128" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K128" s="41"/>
+      <c r="K128" s="40"/>
     </row>
     <row r="129" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K129" s="41"/>
+      <c r="K129" s="40"/>
     </row>
     <row r="130" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K130" s="41"/>
+      <c r="K130" s="40"/>
     </row>
     <row r="131" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K131" s="41"/>
+      <c r="K131" s="40"/>
     </row>
     <row r="132" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K132" s="41"/>
+      <c r="K132" s="40"/>
     </row>
     <row r="133" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K133" s="41"/>
+      <c r="K133" s="40"/>
     </row>
     <row r="134" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K134" s="41"/>
+      <c r="K134" s="40"/>
     </row>
     <row r="135" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K135" s="41"/>
+      <c r="K135" s="40"/>
     </row>
     <row r="136" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K136" s="41"/>
+      <c r="K136" s="40"/>
     </row>
     <row r="137" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K137" s="41"/>
+      <c r="K137" s="40"/>
     </row>
     <row r="138" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K138" s="41"/>
+      <c r="K138" s="40"/>
     </row>
     <row r="139" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K139" s="41"/>
+      <c r="K139" s="40"/>
     </row>
     <row r="140" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K140" s="41"/>
+      <c r="K140" s="40"/>
     </row>
     <row r="141" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K141" s="41"/>
+      <c r="K141" s="40"/>
     </row>
     <row r="142" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K142" s="41"/>
+      <c r="K142" s="40"/>
     </row>
     <row r="143" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K143" s="41"/>
+      <c r="K143" s="40"/>
     </row>
     <row r="144" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K144" s="41"/>
+      <c r="K144" s="40"/>
     </row>
     <row r="145" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K145" s="41"/>
+      <c r="K145" s="40"/>
     </row>
     <row r="146" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K146" s="41"/>
+      <c r="K146" s="40"/>
     </row>
     <row r="147" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K147" s="41"/>
+      <c r="K147" s="40"/>
     </row>
     <row r="148" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K148" s="41"/>
+      <c r="K148" s="40"/>
     </row>
     <row r="149" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K149" s="41"/>
+      <c r="K149" s="40"/>
     </row>
     <row r="150" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K150" s="41"/>
+      <c r="K150" s="40"/>
     </row>
     <row r="151" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K151" s="41"/>
+      <c r="K151" s="40"/>
     </row>
     <row r="152" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K152" s="41"/>
+      <c r="K152" s="40"/>
     </row>
     <row r="153" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K153" s="41"/>
+      <c r="K153" s="40"/>
     </row>
     <row r="154" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K154" s="41"/>
+      <c r="K154" s="40"/>
     </row>
     <row r="155" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K155" s="41"/>
+      <c r="K155" s="40"/>
     </row>
     <row r="156" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K156" s="41"/>
+      <c r="K156" s="40"/>
     </row>
     <row r="157" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K157" s="41"/>
+      <c r="K157" s="40"/>
     </row>
     <row r="158" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K158" s="41"/>
+      <c r="K158" s="40"/>
     </row>
     <row r="159" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K159" s="41"/>
+      <c r="K159" s="40"/>
     </row>
     <row r="160" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K160" s="41"/>
+      <c r="K160" s="40"/>
     </row>
     <row r="161" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K161" s="41"/>
+      <c r="K161" s="40"/>
     </row>
     <row r="162" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K162" s="41"/>
+      <c r="K162" s="40"/>
     </row>
     <row r="163" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K163" s="41"/>
+      <c r="K163" s="40"/>
     </row>
     <row r="164" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K164" s="41"/>
+      <c r="K164" s="40"/>
     </row>
     <row r="165" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K165" s="41"/>
+      <c r="K165" s="40"/>
     </row>
     <row r="166" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K166" s="41"/>
+      <c r="K166" s="40"/>
     </row>
     <row r="167" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K167" s="41"/>
+      <c r="K167" s="40"/>
     </row>
     <row r="168" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K168" s="41"/>
+      <c r="K168" s="40"/>
     </row>
     <row r="169" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K169" s="41"/>
+      <c r="K169" s="40"/>
     </row>
     <row r="170" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K170" s="41"/>
+      <c r="K170" s="40"/>
     </row>
     <row r="171" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K171" s="41"/>
+      <c r="K171" s="40"/>
     </row>
     <row r="172" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K172" s="41"/>
+      <c r="K172" s="40"/>
     </row>
     <row r="173" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K173" s="41"/>
+      <c r="K173" s="40"/>
     </row>
     <row r="174" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K174" s="41"/>
+      <c r="K174" s="40"/>
     </row>
     <row r="175" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K175" s="41"/>
+      <c r="K175" s="40"/>
     </row>
     <row r="176" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K176" s="41"/>
+      <c r="K176" s="40"/>
     </row>
     <row r="177" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K177" s="41"/>
+      <c r="K177" s="40"/>
     </row>
     <row r="178" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K178" s="41"/>
+      <c r="K178" s="40"/>
     </row>
     <row r="179" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K179" s="41"/>
+      <c r="K179" s="40"/>
     </row>
     <row r="180" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K180" s="41"/>
+      <c r="K180" s="40"/>
     </row>
     <row r="181" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K181" s="41"/>
+      <c r="K181" s="40"/>
     </row>
     <row r="182" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K182" s="41"/>
+      <c r="K182" s="40"/>
     </row>
     <row r="183" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K183" s="41"/>
+      <c r="K183" s="40"/>
     </row>
     <row r="184" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K184" s="41"/>
+      <c r="K184" s="40"/>
     </row>
     <row r="185" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K185" s="41"/>
+      <c r="K185" s="40"/>
     </row>
     <row r="186" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K186" s="41"/>
+      <c r="K186" s="40"/>
     </row>
     <row r="187" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K187" s="41"/>
+      <c r="K187" s="40"/>
     </row>
     <row r="188" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K188" s="41"/>
+      <c r="K188" s="40"/>
     </row>
     <row r="189" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K189" s="41"/>
+      <c r="K189" s="40"/>
     </row>
     <row r="190" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K190" s="41"/>
+      <c r="K190" s="40"/>
     </row>
     <row r="191" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K191" s="41"/>
+      <c r="K191" s="40"/>
     </row>
     <row r="192" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K192" s="41"/>
+      <c r="K192" s="40"/>
     </row>
     <row r="193" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K193" s="41"/>
+      <c r="K193" s="40"/>
     </row>
     <row r="194" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K194" s="41"/>
+      <c r="K194" s="40"/>
     </row>
     <row r="195" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K195" s="41"/>
+      <c r="K195" s="40"/>
     </row>
     <row r="196" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K196" s="41"/>
+      <c r="K196" s="40"/>
     </row>
     <row r="197" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K197" s="41"/>
+      <c r="K197" s="40"/>
     </row>
     <row r="198" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K198" s="41"/>
+      <c r="K198" s="40"/>
     </row>
     <row r="199" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K199" s="41"/>
+      <c r="K199" s="40"/>
     </row>
     <row r="200" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K200" s="41"/>
+      <c r="K200" s="40"/>
     </row>
     <row r="201" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K201" s="41"/>
+      <c r="K201" s="40"/>
     </row>
     <row r="202" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K202" s="41"/>
+      <c r="K202" s="40"/>
     </row>
     <row r="203" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K203" s="41"/>
+      <c r="K203" s="40"/>
     </row>
     <row r="204" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K204" s="41"/>
+      <c r="K204" s="40"/>
     </row>
     <row r="205" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K205" s="41"/>
+      <c r="K205" s="40"/>
     </row>
     <row r="206" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K206" s="41"/>
+      <c r="K206" s="40"/>
     </row>
     <row r="207" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K207" s="41"/>
+      <c r="K207" s="40"/>
     </row>
     <row r="208" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K208" s="41"/>
+      <c r="K208" s="40"/>
     </row>
     <row r="209" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K209" s="41"/>
+      <c r="K209" s="40"/>
     </row>
     <row r="210" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K210" s="41"/>
+      <c r="K210" s="40"/>
     </row>
     <row r="211" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K211" s="41"/>
+      <c r="K211" s="40"/>
     </row>
     <row r="212" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K212" s="41"/>
+      <c r="K212" s="40"/>
     </row>
     <row r="213" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K213" s="41"/>
+      <c r="K213" s="40"/>
     </row>
     <row r="214" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K214" s="41"/>
+      <c r="K214" s="40"/>
     </row>
     <row r="215" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K215" s="41"/>
+      <c r="K215" s="40"/>
     </row>
     <row r="216" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K216" s="41"/>
+      <c r="K216" s="40"/>
     </row>
     <row r="217" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K217" s="41"/>
+      <c r="K217" s="40"/>
     </row>
     <row r="218" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K218" s="41"/>
+      <c r="K218" s="40"/>
     </row>
     <row r="219" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K219" s="41"/>
+      <c r="K219" s="40"/>
     </row>
     <row r="220" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K220" s="41"/>
+      <c r="K220" s="40"/>
     </row>
     <row r="221" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K221" s="41"/>
+      <c r="K221" s="40"/>
     </row>
     <row r="222" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K222" s="41"/>
+      <c r="K222" s="40"/>
     </row>
     <row r="223" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K223" s="41"/>
+      <c r="K223" s="40"/>
     </row>
     <row r="224" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K224" s="41"/>
+      <c r="K224" s="40"/>
     </row>
     <row r="225" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K225" s="41"/>
+      <c r="K225" s="40"/>
     </row>
     <row r="226" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K226" s="41"/>
+      <c r="K226" s="40"/>
     </row>
     <row r="227" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K227" s="41"/>
+      <c r="K227" s="40"/>
     </row>
     <row r="228" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K228" s="41"/>
+      <c r="K228" s="40"/>
     </row>
     <row r="229" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K229" s="41"/>
+      <c r="K229" s="40"/>
     </row>
     <row r="230" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K230" s="41"/>
+      <c r="K230" s="40"/>
     </row>
     <row r="231" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K231" s="41"/>
+      <c r="K231" s="40"/>
     </row>
     <row r="232" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K232" s="41"/>
+      <c r="K232" s="40"/>
     </row>
     <row r="233" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K233" s="41"/>
+      <c r="K233" s="40"/>
     </row>
     <row r="234" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K234" s="41"/>
+      <c r="K234" s="40"/>
     </row>
     <row r="235" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K235" s="41"/>
+      <c r="K235" s="40"/>
     </row>
     <row r="236" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K236" s="41"/>
+      <c r="K236" s="40"/>
     </row>
     <row r="237" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K237" s="41"/>
+      <c r="K237" s="40"/>
     </row>
     <row r="238" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K238" s="41"/>
+      <c r="K238" s="40"/>
     </row>
     <row r="239" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K239" s="41"/>
+      <c r="K239" s="40"/>
     </row>
     <row r="240" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K240" s="41"/>
+      <c r="K240" s="40"/>
     </row>
     <row r="241" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K241" s="41"/>
+      <c r="K241" s="40"/>
     </row>
     <row r="242" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K242" s="41"/>
+      <c r="K242" s="40"/>
     </row>
     <row r="243" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K243" s="41"/>
+      <c r="K243" s="40"/>
     </row>
     <row r="244" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K244" s="41"/>
+      <c r="K244" s="40"/>
     </row>
     <row r="245" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K245" s="41"/>
+      <c r="K245" s="40"/>
     </row>
     <row r="246" spans="11:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K246" s="41"/>
+      <c r="K246" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>